<commit_message>
Update mapping and OWL annotations
Updated some of the mapping files
Mainly created new entries for matching annotations rather than using the new line to store all in one entry
</commit_message>
<xml_diff>
--- a/Avantis Mapping/SPARQL_category.xlsx
+++ b/Avantis Mapping/SPARQL_category.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medney\Documents\GitHub\TWONTO\Avantis Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{843277E6-CF42-4725-A01C-1DA5BB2AF6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DC7112-BD60-4518-8089-E58BC443A36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{716C0CF8-2E33-46F2-BE6F-578AC5702A19}"/>
   </bookViews>
@@ -36,335 +36,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="337">
   <si>
     <t>TWONTO</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#cable_segment</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#humidier</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#chlorinator_system</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#ozone_generator</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#gearbox</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#clarifier</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#instrument_element</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#channel_gate</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#600V_insulated_case_electrical_cabinet</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#security_camera</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#public_annoucement_speaker</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#dehumidifier</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#crane</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#engine</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#rupture_disc</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#pipe_segment</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#chiller</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#centrifuge</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#auto_sampler</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#automatic_external_defibrillator</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#elevator</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#self-contained_breathing_apparatus</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#level_switch</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#temperature_transmitter</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#weight_scale</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#manhole</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#roll_up_door</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#UV_disinfection_assembly</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#transformer</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#fixed_gas_detector</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#slude_density_meter</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#strainer</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#valve</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#air_scrubber</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#grinder_or_comminutor</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#air_condition</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#120V-208V_electrical_panel</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#heat_exchanger</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#computer</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#SCADA_computer_terminal</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#instrument_transmitter</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#temperature_sensor_element</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#position_sensing_instrument</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#classifier</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#flame_arrestor</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#outfall_or_discharge_point</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#5kV_electrical_cabinet</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#dust_collector</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#fire_rated_door</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#pressure_transmitter</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#screen</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#mixer_or_agitator</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#UPS</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#reservoir_tank</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#flow_transmitter</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#flow_switch</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#heater</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#generator-set</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#well</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#collector_mechanism</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#capacitor</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#level_sensor_element</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#compactor</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#blower</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#controller</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#pump_-_without_drive</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#controlled_door_access</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#server_appliance</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#motor</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#protection_relay</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#process_control_panel</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#ash_lagoon</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#storage_tank</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#welding_receptacle</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#vibration_analyzer</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#RTU</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#compressor</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#air_damper</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#motor_starter</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#spill_kit</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#torque_switch</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#boiler</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#conveyor</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#equipment_or_access_chamber</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#hydraulic_power_pack</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#large_stationary_tool</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#level_transmitter</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#backflow_preventer</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#annunciator_panel</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#first_aid_kit</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#data_logger</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#breaker</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#pressure_switch</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#position_switch</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#temperature_switch</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#electrical_current_sensing_instrument</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#lighting_unit</t>
   </si>
   <si>
     <t>UPS_x000D_
 Uninterruptible Power Supply</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#rotating_collector</t>
-  </si>
-  <si>
     <t>Collector,Circular_x000D_
 Collector,Helical Rotating</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#planer</t>
-  </si>
-  <si>
     <t>Machine Tool,Planer</t>
   </si>
   <si>
     <t>Controller</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#flocculation_tank</t>
-  </si>
-  <si>
     <t>Flocculator</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#security_motion_sensor</t>
-  </si>
-  <si>
     <t>Sensor,Security</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#fall_protection_energy_absorber</t>
   </si>
   <si>
     <t>PPE,Lanyard</t>
@@ -374,9 +68,6 @@
 Relay,Protective</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#mass_flow_meter</t>
-  </si>
-  <si>
     <t>Meter,Flow,Mass</t>
   </si>
   <si>
@@ -384,9 +75,6 @@
   </si>
   <si>
     <t>Maintenance Hole</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#PLC</t>
   </si>
   <si>
     <t>Controller,PLC</t>
@@ -399,9 +87,6 @@
 Dust Control,Odour Control</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#pressure_sensor_element</t>
-  </si>
-  <si>
     <t>Pressure Sensor_x000D_
 Sensor,Pressure</t>
   </si>
@@ -421,9 +106,6 @@
     <t>Door,Overhead</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#ozone_analyzer</t>
-  </si>
-  <si>
     <t>Analyzer,Ozone</t>
   </si>
   <si>
@@ -439,15 +121,9 @@
     <t>Sensor,Level</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#jointer</t>
-  </si>
-  <si>
     <t>Machine Tool,Jointer</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#UV_disinfection_lamp_unit</t>
-  </si>
-  <si>
     <t>Ultraviolet Disinfection,Bank</t>
   </si>
   <si>
@@ -457,16 +133,10 @@
     <t>Tank</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#radial_arm_drill</t>
-  </si>
-  <si>
     <t>Machine Tool,Radial arm Drill</t>
   </si>
   <si>
     <t>Flame Arrester</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#cyclone_classifier</t>
   </si>
   <si>
     <t>Cyclone_x000D_
@@ -487,9 +157,6 @@
     <t>Safety, First Aid Kit</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#lifting_equipment_hoist</t>
-  </si>
-  <si>
     <t>Lifting Device,Hoist</t>
   </si>
   <si>
@@ -501,9 +168,6 @@
 Starter</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#network_switch</t>
-  </si>
-  <si>
     <t>Network,Switch</t>
   </si>
   <si>
@@ -514,9 +178,6 @@
 Door</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#VSD</t>
-  </si>
-  <si>
     <t>Drive,Variable Speed Electrical_x000D_
 Drive,Variable Speed Mechanical</t>
   </si>
@@ -531,61 +192,37 @@
     <t>Spill Kit</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#ultraviolet_analyzer</t>
-  </si>
-  <si>
     <t>Analyzer,UV</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#still_or_video_mobile_camera</t>
-  </si>
-  <si>
     <t>Camera</t>
   </si>
   <si>
     <t>Tank,Reservoir</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#forklift</t>
-  </si>
-  <si>
     <t>Forklift</t>
   </si>
   <si>
     <t>Valve</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#VFD</t>
-  </si>
-  <si>
     <t>Variable Frequency Drive</t>
   </si>
   <si>
     <t>Electrical Power Line</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#turbidity_analyzer</t>
-  </si>
-  <si>
     <t>Analyzer,Turbidity</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#cooling_tower</t>
-  </si>
-  <si>
     <t>H.V.A.C.,Cooling Tower</t>
   </si>
   <si>
     <t>Chamber</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#ventilation_system</t>
-  </si>
-  <si>
     <t>H.V.A.C.</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#vacuum_cleaner</t>
   </si>
   <si>
     <t>Vacuum</t>
@@ -595,22 +232,13 @@
 Generator,Chlorine</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#belt_conveyor</t>
-  </si>
-  <si>
     <t>Conveyor,Belt</t>
   </si>
   <si>
     <t>Outfall</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#network_router</t>
-  </si>
-  <si>
     <t>Network,Hubs</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#relief_valve</t>
   </si>
   <si>
     <t>Valve,Pressure Relief</t>
@@ -620,9 +248,6 @@
 Sludge Collector</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#motion_sensor_element</t>
-  </si>
-  <si>
     <t>Sensor,Motion_x000D_
 Switch,Motion</t>
   </si>
@@ -633,15 +258,9 @@
     <t>Circuit Breaker</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#sulphite_analyzer</t>
-  </si>
-  <si>
     <t>Analyzer,Residual Sulphite</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#chloramination_analyzer</t>
-  </si>
-  <si>
     <t>Analyzer,Chloramination</t>
   </si>
   <si>
@@ -654,25 +273,13 @@
     <t>Motor</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#orp_analyzer</t>
-  </si>
-  <si>
     <t>Analyzer,ORP</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#milling_machine</t>
-  </si>
-  <si>
     <t>Machine Tool,Milling Machine</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#differential_pressure</t>
-  </si>
-  <si>
     <t>Meter,Flow,Differential Pressure</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#chain_and_flight_collector</t>
   </si>
   <si>
     <t>Collector,Chain and Flight</t>
@@ -688,9 +295,6 @@
     <t>Public Address System</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#pressure_vessel</t>
-  </si>
-  <si>
     <t>Vessel_x000D_
 Vessel,Pressure</t>
   </si>
@@ -708,37 +312,22 @@
     <t>Electrical Power Line,Welding Receptable</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#boat</t>
-  </si>
-  <si>
     <t>Boat</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#actuator</t>
-  </si>
-  <si>
     <t>Actuator</t>
   </si>
   <si>
     <t>Engine</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#sludge_blanket_analyzer</t>
-  </si>
-  <si>
     <t>Meter,Sludge Blanket</t>
   </si>
   <si>
     <t>Pump</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#passenger_vehicles</t>
-  </si>
-  <si>
     <t>Vehicle</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#safety_valve</t>
   </si>
   <si>
     <t>Valve,Safety_x000D_
@@ -749,16 +338,10 @@
 Valve,Backflow Preventer,Reduced Pressure</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#PH_analyzer</t>
-  </si>
-  <si>
     <t>Analyzer,PH</t>
   </si>
   <si>
     <t>Transmitter,Vibration</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#lathe</t>
   </si>
   <si>
     <t>Machine Tool,Lathe</t>
@@ -772,36 +355,24 @@
 Meter,Power Recording</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#dissolved_oxygen_analyzer</t>
-  </si>
-  <si>
     <t>Analyzer,Dissolved Oxygen (DO)</t>
   </si>
   <si>
     <t>Piping</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#screw_conveyor</t>
-  </si>
-  <si>
     <t>Conveyor,Screw</t>
   </si>
   <si>
     <t>Transmitter,Pressure</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#incinerator</t>
-  </si>
-  <si>
     <t>Incinerator</t>
   </si>
   <si>
     <t>Damper/Louver</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#drill_press</t>
-  </si>
-  <si>
     <t>Machine Tool,Drill Press</t>
   </si>
   <si>
@@ -811,9 +382,6 @@
     <t>Centrifuge</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#dryer</t>
-  </si>
-  <si>
     <t>Drier</t>
   </si>
   <si>
@@ -823,16 +391,10 @@
     <t>Control Panel</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#rubber_insulating_gloves</t>
-  </si>
-  <si>
     <t>PPE,Insulated Glove</t>
   </si>
   <si>
     <t>Sampler</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#total_suspended_solids_analyzer</t>
   </si>
   <si>
     <t>Analyzer,Suspended Solid_x000D_
@@ -843,9 +405,6 @@
 Heater</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#positive_displacement_flow_elements</t>
-  </si>
-  <si>
     <t>Meter,Flow,Displacement</t>
   </si>
   <si>
@@ -865,13 +424,7 @@
     <t>Sensor</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#position_transmitter</t>
-  </si>
-  <si>
     <t>Transmitter,Position</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#travelling_bridge_collector</t>
   </si>
   <si>
     <t>Collector,Bridge</t>
@@ -881,16 +434,10 @@
 Atmosphere Monitoring Device</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#ultrasonic_flow_meter</t>
-  </si>
-  <si>
     <t>Meter,Flow,Doppler_x000D_
 Meter,Flow,Ultrasonic</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#ammonia_analyzer</t>
-  </si>
-  <si>
     <t>Analyzer,Ammonia</t>
   </si>
   <si>
@@ -910,9 +457,6 @@
   </si>
   <si>
     <t>Compressor</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#table_saw</t>
   </si>
   <si>
     <t>Machine Tool,Table Saw</t>
@@ -945,15 +489,9 @@
     <t>H.V.A.C.,Dehumidifier</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#elevated_water_tank</t>
-  </si>
-  <si>
     <t>Tank,Water Elevated</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#magmeter</t>
-  </si>
-  <si>
     <t>Meter,Flow,Magmeter</t>
   </si>
   <si>
@@ -966,18 +504,9 @@
     <t>Security System,Camera</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#intercom_unit</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#hot_water_tank</t>
-  </si>
-  <si>
     <t>Domestic Hot Water</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#venturi</t>
-  </si>
-  <si>
     <t>Meter,Flow,Venturi</t>
   </si>
   <si>
@@ -987,22 +516,13 @@
     <t>Switch,Torque</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#chlorine_analyzer</t>
-  </si>
-  <si>
     <t>Analyzer,Chlorine</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#orthophosphate_analyzer</t>
-  </si>
-  <si>
     <t>Analyzer,Orthophosphate</t>
   </si>
   <si>
     <t>Lagoon</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#fall_arrest_harness</t>
   </si>
   <si>
     <t>PPE,Harness</t>
@@ -1012,13 +532,7 @@
 Meter,Temperature</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#fluoride_analyzer</t>
-  </si>
-  <si>
     <t>Analyzer,Fluoride</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#check_valve</t>
   </si>
   <si>
     <t>Valve,Check</t>
@@ -1038,9 +552,6 @@
     <t>Control Panel,Lighting</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#flow_sensor_element</t>
-  </si>
-  <si>
     <t>Sensor,Flow</t>
   </si>
   <si>
@@ -1051,36 +562,21 @@
   </si>
   <si>
     <t>Transformer</t>
-  </si>
-  <si>
-    <t>http://www.toronto.ca/TWONTO#emergency_eyewash</t>
   </si>
   <si>
     <t>PPE,Eyewash Station_x000D_
 Safety, Eye wash</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#gas_holder</t>
-  </si>
-  <si>
     <t>Gas Well</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#granular_material</t>
-  </si>
-  <si>
     <t>Filter</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#bar_screen_unit</t>
-  </si>
-  <si>
     <t>Screen,Bar</t>
   </si>
   <si>
-    <t>http://www.toronto.ca/TWONTO#screw_classifier</t>
-  </si>
-  <si>
     <t>Classifier,Incline Screw</t>
   </si>
   <si>
@@ -1088,6 +584,507 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>UPS</t>
+  </si>
+  <si>
+    <t>rotating_collector</t>
+  </si>
+  <si>
+    <t>planer</t>
+  </si>
+  <si>
+    <t>controller</t>
+  </si>
+  <si>
+    <t>flocculation_tank</t>
+  </si>
+  <si>
+    <t>security_motion_sensor</t>
+  </si>
+  <si>
+    <t>fall_protection_energy_absorber</t>
+  </si>
+  <si>
+    <t>protection_relay</t>
+  </si>
+  <si>
+    <t>mass_flow_meter</t>
+  </si>
+  <si>
+    <t>automatic_external_defibrillator</t>
+  </si>
+  <si>
+    <t>manhole</t>
+  </si>
+  <si>
+    <t>PLC</t>
+  </si>
+  <si>
+    <t>temperature_switch</t>
+  </si>
+  <si>
+    <t>dust_collector</t>
+  </si>
+  <si>
+    <t>pressure_sensor_element</t>
+  </si>
+  <si>
+    <t>RTU</t>
+  </si>
+  <si>
+    <t>flow_switch</t>
+  </si>
+  <si>
+    <t>large_stationary_tool</t>
+  </si>
+  <si>
+    <t>computer</t>
+  </si>
+  <si>
+    <t>roll_up_door</t>
+  </si>
+  <si>
+    <t>ozone_analyzer</t>
+  </si>
+  <si>
+    <t>level_switch</t>
+  </si>
+  <si>
+    <t>elevator</t>
+  </si>
+  <si>
+    <t>fire_rated_door</t>
+  </si>
+  <si>
+    <t>level_sensor_element</t>
+  </si>
+  <si>
+    <t>jointer</t>
+  </si>
+  <si>
+    <t>UV_disinfection_lamp_unit</t>
+  </si>
+  <si>
+    <t>air_scrubber</t>
+  </si>
+  <si>
+    <t>storage_tank</t>
+  </si>
+  <si>
+    <t>radial_arm_drill</t>
+  </si>
+  <si>
+    <t>flame_arrestor</t>
+  </si>
+  <si>
+    <t>cyclone_classifier</t>
+  </si>
+  <si>
+    <t>slude_density_meter</t>
+  </si>
+  <si>
+    <t>generator-set</t>
+  </si>
+  <si>
+    <t>instrument_transmitter</t>
+  </si>
+  <si>
+    <t>first_aid_kit</t>
+  </si>
+  <si>
+    <t>lifting_equipment_hoist</t>
+  </si>
+  <si>
+    <t>mixer_or_agitator</t>
+  </si>
+  <si>
+    <t>motor_starter</t>
+  </si>
+  <si>
+    <t>network_switch</t>
+  </si>
+  <si>
+    <t>weight_scale</t>
+  </si>
+  <si>
+    <t>controlled_door_access</t>
+  </si>
+  <si>
+    <t>VSD</t>
+  </si>
+  <si>
+    <t>UV_disinfection_assembly</t>
+  </si>
+  <si>
+    <t>flow_transmitter</t>
+  </si>
+  <si>
+    <t>spill_kit</t>
+  </si>
+  <si>
+    <t>ultraviolet_analyzer</t>
+  </si>
+  <si>
+    <t>still_or_video_mobile_camera</t>
+  </si>
+  <si>
+    <t>reservoir_tank</t>
+  </si>
+  <si>
+    <t>forklift</t>
+  </si>
+  <si>
+    <t>valve</t>
+  </si>
+  <si>
+    <t>VFD</t>
+  </si>
+  <si>
+    <t>cable_segment</t>
+  </si>
+  <si>
+    <t>turbidity_analyzer</t>
+  </si>
+  <si>
+    <t>cooling_tower</t>
+  </si>
+  <si>
+    <t>equipment_or_access_chamber</t>
+  </si>
+  <si>
+    <t>ventilation_system</t>
+  </si>
+  <si>
+    <t>vacuum_cleaner</t>
+  </si>
+  <si>
+    <t>chlorinator_system</t>
+  </si>
+  <si>
+    <t>belt_conveyor</t>
+  </si>
+  <si>
+    <t>outfall_or_discharge_point</t>
+  </si>
+  <si>
+    <t>network_router</t>
+  </si>
+  <si>
+    <t>relief_valve</t>
+  </si>
+  <si>
+    <t>collector_mechanism</t>
+  </si>
+  <si>
+    <t>motion_sensor_element</t>
+  </si>
+  <si>
+    <t>boiler</t>
+  </si>
+  <si>
+    <t>breaker</t>
+  </si>
+  <si>
+    <t>sulphite_analyzer</t>
+  </si>
+  <si>
+    <t>chloramination_analyzer</t>
+  </si>
+  <si>
+    <t>classifier</t>
+  </si>
+  <si>
+    <t>annunciator_panel</t>
+  </si>
+  <si>
+    <t>motor</t>
+  </si>
+  <si>
+    <t>orp_analyzer</t>
+  </si>
+  <si>
+    <t>milling_machine</t>
+  </si>
+  <si>
+    <t>differential_pressure</t>
+  </si>
+  <si>
+    <t>chain_and_flight_collector</t>
+  </si>
+  <si>
+    <t>level_transmitter</t>
+  </si>
+  <si>
+    <t>capacitor</t>
+  </si>
+  <si>
+    <t>public_annoucement_speaker</t>
+  </si>
+  <si>
+    <t>pressure_vessel</t>
+  </si>
+  <si>
+    <t>air_condition</t>
+  </si>
+  <si>
+    <t>hydraulic_power_pack</t>
+  </si>
+  <si>
+    <t>heat_exchanger</t>
+  </si>
+  <si>
+    <t>welding_receptacle</t>
+  </si>
+  <si>
+    <t>boat</t>
+  </si>
+  <si>
+    <t>actuator</t>
+  </si>
+  <si>
+    <t>engine</t>
+  </si>
+  <si>
+    <t>sludge_blanket_analyzer</t>
+  </si>
+  <si>
+    <t>pump_-_without_drive</t>
+  </si>
+  <si>
+    <t>passenger_vehicles</t>
+  </si>
+  <si>
+    <t>safety_valve</t>
+  </si>
+  <si>
+    <t>backflow_preventer</t>
+  </si>
+  <si>
+    <t>PH_analyzer</t>
+  </si>
+  <si>
+    <t>vibration_analyzer</t>
+  </si>
+  <si>
+    <t>lathe</t>
+  </si>
+  <si>
+    <t>blower</t>
+  </si>
+  <si>
+    <t>electrical_current_sensing_instrument</t>
+  </si>
+  <si>
+    <t>dissolved_oxygen_analyzer</t>
+  </si>
+  <si>
+    <t>pipe_segment</t>
+  </si>
+  <si>
+    <t>screw_conveyor</t>
+  </si>
+  <si>
+    <t>pressure_transmitter</t>
+  </si>
+  <si>
+    <t>incinerator</t>
+  </si>
+  <si>
+    <t>air_damper</t>
+  </si>
+  <si>
+    <t>drill_press</t>
+  </si>
+  <si>
+    <t>pressure_switch</t>
+  </si>
+  <si>
+    <t>centrifuge</t>
+  </si>
+  <si>
+    <t>dryer</t>
+  </si>
+  <si>
+    <t>SCADA_computer_terminal</t>
+  </si>
+  <si>
+    <t>process_control_panel</t>
+  </si>
+  <si>
+    <t>rubber_insulating_gloves</t>
+  </si>
+  <si>
+    <t>auto_sampler</t>
+  </si>
+  <si>
+    <t>total_suspended_solids_analyzer</t>
+  </si>
+  <si>
+    <t>heater</t>
+  </si>
+  <si>
+    <t>positive_displacement_flow_elements</t>
+  </si>
+  <si>
+    <t>clarifier</t>
+  </si>
+  <si>
+    <t>grinder_or_comminutor</t>
+  </si>
+  <si>
+    <t>600V_insulated_case_electrical_cabinet</t>
+  </si>
+  <si>
+    <t>screen</t>
+  </si>
+  <si>
+    <t>instrument_element</t>
+  </si>
+  <si>
+    <t>position_transmitter</t>
+  </si>
+  <si>
+    <t>travelling_bridge_collector</t>
+  </si>
+  <si>
+    <t>fixed_gas_detector</t>
+  </si>
+  <si>
+    <t>ultrasonic_flow_meter</t>
+  </si>
+  <si>
+    <t>ammonia_analyzer</t>
+  </si>
+  <si>
+    <t>rupture_disc</t>
+  </si>
+  <si>
+    <t>server_appliance</t>
+  </si>
+  <si>
+    <t>ozone_generator</t>
+  </si>
+  <si>
+    <t>chiller</t>
+  </si>
+  <si>
+    <t>5kV_electrical_cabinet</t>
+  </si>
+  <si>
+    <t>compressor</t>
+  </si>
+  <si>
+    <t>table_saw</t>
+  </si>
+  <si>
+    <t>channel_gate</t>
+  </si>
+  <si>
+    <t>crane</t>
+  </si>
+  <si>
+    <t>self-contained_breathing_apparatus</t>
+  </si>
+  <si>
+    <t>conveyor</t>
+  </si>
+  <si>
+    <t>lighting_unit</t>
+  </si>
+  <si>
+    <t>dehumidifier</t>
+  </si>
+  <si>
+    <t>elevated_water_tank</t>
+  </si>
+  <si>
+    <t>magmeter</t>
+  </si>
+  <si>
+    <t>compactor</t>
+  </si>
+  <si>
+    <t>temperature_sensor_element</t>
+  </si>
+  <si>
+    <t>security_camera</t>
+  </si>
+  <si>
+    <t>hot_water_tank</t>
+  </si>
+  <si>
+    <t>venturi</t>
+  </si>
+  <si>
+    <t>strainer</t>
+  </si>
+  <si>
+    <t>torque_switch</t>
+  </si>
+  <si>
+    <t>chlorine_analyzer</t>
+  </si>
+  <si>
+    <t>orthophosphate_analyzer</t>
+  </si>
+  <si>
+    <t>ash_lagoon</t>
+  </si>
+  <si>
+    <t>fall_arrest_harness</t>
+  </si>
+  <si>
+    <t>temperature_transmitter</t>
+  </si>
+  <si>
+    <t>fluoride_analyzer</t>
+  </si>
+  <si>
+    <t>check_valve</t>
+  </si>
+  <si>
+    <t>position_switch</t>
+  </si>
+  <si>
+    <t>gearbox</t>
+  </si>
+  <si>
+    <t>data_logger</t>
+  </si>
+  <si>
+    <t>120V-208V_electrical_panel</t>
+  </si>
+  <si>
+    <t>flow_sensor_element</t>
+  </si>
+  <si>
+    <t>humidier</t>
+  </si>
+  <si>
+    <t>well</t>
+  </si>
+  <si>
+    <t>transformer</t>
+  </si>
+  <si>
+    <t>emergency_eyewash</t>
+  </si>
+  <si>
+    <t>gas_holder</t>
+  </si>
+  <si>
+    <t>granular_material</t>
+  </si>
+  <si>
+    <t>bar_screen_unit</t>
+  </si>
+  <si>
+    <t>screw_classifier</t>
+  </si>
+  <si>
+    <t>position_sensing_instrument</t>
   </si>
 </sst>
 </file>
@@ -1203,8 +1200,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{95B7462F-2E77-4297-9361-348E17AE61B7}" name="Table1" displayName="Table1" ref="A2:B171" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A2:B171" xr:uid="{95B7462F-2E77-4297-9361-348E17AE61B7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{95B7462F-2E77-4297-9361-348E17AE61B7}" name="Table1" displayName="Table1" ref="A2:B170" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A2:B170" xr:uid="{95B7462F-2E77-4297-9361-348E17AE61B7}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{F929C49D-2775-4718-8C6D-B5829C8CADDE}" name="TWONTO"/>
     <tableColumn id="2" xr3:uid="{69FF631B-786D-4A8E-A604-FCCAC8BACC05}" name="Category"/>
@@ -1510,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C799550E-49B1-4512-9CC1-86876BA1337E}">
-  <dimension ref="A2:B171"/>
+  <dimension ref="A2:B170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1527,1359 +1524,1351 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>170</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>171</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>172</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>102</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>103</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>174</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>105</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>176</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>177</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>178</v>
       </c>
       <c r="B11" t="s">
-        <v>112</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>180</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>114</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>181</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>116</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>182</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>183</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>184</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>120</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>185</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>186</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>122</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>187</v>
       </c>
       <c r="B20" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>188</v>
       </c>
       <c r="B21" t="s">
-        <v>124</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>189</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>125</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>190</v>
       </c>
       <c r="B23" t="s">
-        <v>127</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>191</v>
       </c>
       <c r="B24" t="s">
-        <v>128</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>192</v>
       </c>
       <c r="B25" t="s">
-        <v>129</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>193</v>
       </c>
       <c r="B26" t="s">
-        <v>130</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>194</v>
       </c>
       <c r="B27" t="s">
-        <v>131</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>132</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s">
-        <v>133</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="B29" t="s">
-        <v>135</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>197</v>
       </c>
       <c r="B30" t="s">
-        <v>136</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>198</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>137</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>138</v>
+        <v>199</v>
       </c>
       <c r="B32" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>200</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>141</v>
+        <v>201</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>202</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>203</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>144</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>204</v>
       </c>
       <c r="B37" t="s">
-        <v>145</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>90</v>
+        <v>205</v>
       </c>
       <c r="B38" t="s">
-        <v>146</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>147</v>
+        <v>206</v>
       </c>
       <c r="B39" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>207</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>208</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>150</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>151</v>
+        <v>209</v>
       </c>
       <c r="B42" t="s">
-        <v>152</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>210</v>
       </c>
       <c r="B43" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>211</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>213</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>157</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>214</v>
       </c>
       <c r="B47" t="s">
-        <v>158</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>80</v>
+        <v>215</v>
       </c>
       <c r="B48" t="s">
-        <v>159</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>160</v>
+        <v>216</v>
       </c>
       <c r="B49" t="s">
-        <v>161</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>162</v>
+        <v>217</v>
       </c>
       <c r="B50" t="s">
-        <v>163</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>218</v>
       </c>
       <c r="B51" t="s">
-        <v>164</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>165</v>
+        <v>219</v>
       </c>
       <c r="B52" t="s">
-        <v>166</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>33</v>
+        <v>220</v>
       </c>
       <c r="B53" t="s">
-        <v>167</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>168</v>
+        <v>221</v>
       </c>
       <c r="B54" t="s">
-        <v>169</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>1</v>
+        <v>222</v>
       </c>
       <c r="B55" t="s">
-        <v>170</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>171</v>
+        <v>223</v>
       </c>
       <c r="B56" t="s">
-        <v>172</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>173</v>
+        <v>224</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>174</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>225</v>
       </c>
       <c r="B58" t="s">
-        <v>175</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="B59" t="s">
-        <v>177</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>178</v>
+        <v>227</v>
       </c>
       <c r="B60" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>3</v>
+        <v>228</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>180</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>181</v>
+        <v>229</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>182</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>46</v>
+        <v>230</v>
       </c>
       <c r="B63" t="s">
-        <v>183</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>184</v>
+        <v>231</v>
       </c>
       <c r="B64" t="s">
-        <v>185</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>186</v>
+        <v>232</v>
       </c>
       <c r="B65" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>233</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>189</v>
+        <v>234</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>190</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>235</v>
       </c>
       <c r="B68" t="s">
-        <v>191</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>92</v>
+        <v>236</v>
       </c>
       <c r="B69" t="s">
-        <v>192</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>193</v>
+        <v>237</v>
       </c>
       <c r="B70" t="s">
-        <v>194</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>195</v>
+        <v>238</v>
       </c>
       <c r="B71" t="s">
-        <v>196</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>44</v>
+        <v>239</v>
       </c>
       <c r="B72" t="s">
-        <v>197</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>89</v>
+        <v>240</v>
       </c>
       <c r="B73" t="s">
-        <v>198</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>241</v>
       </c>
       <c r="B74" t="s">
-        <v>199</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>200</v>
+        <v>242</v>
       </c>
       <c r="B75" t="s">
-        <v>201</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>202</v>
+        <v>243</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>203</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>204</v>
+        <v>244</v>
       </c>
       <c r="B77" t="s">
-        <v>205</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>206</v>
+        <v>245</v>
       </c>
       <c r="B78" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>87</v>
+        <v>246</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>208</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>61</v>
+        <v>247</v>
       </c>
       <c r="B80" t="s">
-        <v>209</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>11</v>
+        <v>248</v>
       </c>
       <c r="B81" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>211</v>
+        <v>249</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>212</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>36</v>
+        <v>250</v>
       </c>
       <c r="B83" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>214</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>38</v>
+        <v>252</v>
       </c>
       <c r="B85" t="s">
-        <v>215</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>74</v>
+        <v>253</v>
       </c>
       <c r="B86" t="s">
-        <v>216</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>217</v>
+        <v>254</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>218</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>219</v>
+        <v>255</v>
       </c>
       <c r="B88" t="s">
-        <v>220</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>256</v>
       </c>
       <c r="B89" t="s">
-        <v>221</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>222</v>
+        <v>257</v>
       </c>
       <c r="B90" t="s">
-        <v>223</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>66</v>
+        <v>258</v>
       </c>
       <c r="B91" t="s">
-        <v>224</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>225</v>
+        <v>259</v>
       </c>
       <c r="B92" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>227</v>
+        <v>260</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>88</v>
+        <v>261</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>229</v>
+        <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>230</v>
+        <v>262</v>
       </c>
       <c r="B95" t="s">
-        <v>231</v>
+        <v>93</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>75</v>
+        <v>263</v>
       </c>
       <c r="B96" t="s">
-        <v>232</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>233</v>
+        <v>264</v>
       </c>
       <c r="B97" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>64</v>
+        <v>265</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>96</v>
+        <v>266</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>236</v>
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>237</v>
+        <v>267</v>
       </c>
       <c r="B100" t="s">
-        <v>238</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>16</v>
+        <v>268</v>
       </c>
       <c r="B101" t="s">
-        <v>239</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>240</v>
+        <v>269</v>
       </c>
       <c r="B102" t="s">
-        <v>241</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>50</v>
+        <v>270</v>
       </c>
       <c r="B103" t="s">
-        <v>242</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
       <c r="B104" t="s">
-        <v>244</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>78</v>
+        <v>272</v>
       </c>
       <c r="B105" t="s">
-        <v>245</v>
+        <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>247</v>
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>93</v>
+        <v>274</v>
       </c>
       <c r="B107" t="s">
-        <v>248</v>
+        <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>18</v>
+        <v>275</v>
       </c>
       <c r="B108" t="s">
-        <v>249</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>250</v>
+        <v>276</v>
       </c>
       <c r="B109" t="s">
-        <v>251</v>
+        <v>107</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>40</v>
+        <v>277</v>
       </c>
       <c r="B110" t="s">
-        <v>252</v>
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>71</v>
+        <v>278</v>
       </c>
       <c r="B111" t="s">
-        <v>253</v>
+        <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>254</v>
+        <v>279</v>
       </c>
       <c r="B112" t="s">
-        <v>255</v>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>19</v>
+        <v>280</v>
       </c>
       <c r="B113" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>57</v>
+        <v>282</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>259</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
       <c r="B116" t="s">
-        <v>261</v>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>6</v>
+        <v>284</v>
       </c>
       <c r="B117" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>35</v>
+        <v>285</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>263</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>9</v>
+        <v>286</v>
       </c>
       <c r="B119" t="s">
-        <v>264</v>
+        <v>117</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>51</v>
+        <v>287</v>
       </c>
       <c r="B120" t="s">
-        <v>265</v>
+        <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>7</v>
+        <v>288</v>
       </c>
       <c r="B121" t="s">
-        <v>266</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>267</v>
+        <v>289</v>
       </c>
       <c r="B122" t="s">
-        <v>268</v>
+        <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>269</v>
+        <v>290</v>
       </c>
       <c r="B123" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>30</v>
+        <v>291</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>273</v>
+        <v>123</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>274</v>
+        <v>293</v>
       </c>
       <c r="B126" t="s">
-        <v>275</v>
+        <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>15</v>
+        <v>294</v>
       </c>
       <c r="B127" t="s">
-        <v>276</v>
+        <v>125</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>68</v>
+        <v>295</v>
       </c>
       <c r="B128" t="s">
-        <v>277</v>
+        <v>126</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>4</v>
+        <v>296</v>
       </c>
       <c r="B129" t="s">
-        <v>278</v>
+        <v>127</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>17</v>
+        <v>297</v>
       </c>
       <c r="B130" t="s">
-        <v>279</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>47</v>
+        <v>298</v>
       </c>
       <c r="B131" t="s">
-        <v>280</v>
+        <v>129</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>77</v>
+        <v>299</v>
       </c>
       <c r="B132" t="s">
-        <v>281</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="B133" t="s">
-        <v>283</v>
+        <v>131</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>80</v>
+        <v>215</v>
       </c>
       <c r="B134" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>8</v>
+        <v>301</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>285</v>
+        <v>133</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>13</v>
+        <v>302</v>
       </c>
       <c r="B136" t="s">
-        <v>286</v>
+        <v>134</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>22</v>
+        <v>303</v>
       </c>
       <c r="B137" t="s">
-        <v>287</v>
+        <v>135</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>83</v>
+        <v>304</v>
       </c>
       <c r="B138" t="s">
-        <v>288</v>
+        <v>136</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>97</v>
+        <v>305</v>
       </c>
       <c r="B139" t="s">
-        <v>289</v>
+        <v>137</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>12</v>
+        <v>306</v>
       </c>
       <c r="B140" t="s">
-        <v>290</v>
+        <v>138</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>291</v>
+        <v>307</v>
       </c>
       <c r="B141" t="s">
-        <v>292</v>
+        <v>139</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="B142" t="s">
-        <v>294</v>
+        <v>140</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>63</v>
+        <v>309</v>
       </c>
       <c r="B143" t="s">
-        <v>295</v>
+        <v>141</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>42</v>
+        <v>310</v>
       </c>
       <c r="B144" t="s">
-        <v>296</v>
+        <v>142</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>10</v>
+        <v>311</v>
       </c>
       <c r="B145" t="s">
-        <v>297</v>
+        <v>143</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>298</v>
+        <v>312</v>
       </c>
       <c r="B146" t="s">
-        <v>210</v>
+        <v>144</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="B147" t="s">
-        <v>300</v>
+        <v>145</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>301</v>
+        <v>314</v>
       </c>
       <c r="B148" t="s">
-        <v>302</v>
+        <v>146</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>32</v>
+        <v>315</v>
       </c>
       <c r="B149" t="s">
-        <v>303</v>
+        <v>147</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>81</v>
+        <v>316</v>
       </c>
       <c r="B150" t="s">
-        <v>304</v>
+        <v>148</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
       <c r="B151" t="s">
-        <v>306</v>
+        <v>149</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="B152" t="s">
-        <v>308</v>
+        <v>150</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>72</v>
+        <v>319</v>
       </c>
       <c r="B153" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>310</v>
-      </c>
-      <c r="B154" t="s">
-        <v>311</v>
+        <v>320</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>24</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>312</v>
+        <v>321</v>
+      </c>
+      <c r="B155" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="B156" t="s">
-        <v>314</v>
+        <v>154</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="B157" t="s">
-        <v>316</v>
+        <v>155</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>94</v>
+        <v>324</v>
       </c>
       <c r="B158" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>5</v>
-      </c>
-      <c r="B159" t="s">
-        <v>318</v>
+        <v>325</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>91</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>319</v>
+        <v>326</v>
+      </c>
+      <c r="B160" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>37</v>
+        <v>327</v>
       </c>
       <c r="B161" t="s">
-        <v>320</v>
+        <v>159</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="B162" t="s">
-        <v>322</v>
+        <v>160</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>2</v>
+        <v>329</v>
       </c>
       <c r="B163" t="s">
-        <v>323</v>
+        <v>161</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>59</v>
+        <v>330</v>
       </c>
       <c r="B164" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>29</v>
-      </c>
-      <c r="B165" t="s">
-        <v>325</v>
+        <v>331</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>326</v>
-      </c>
-      <c r="B166" s="3" t="s">
-        <v>327</v>
+        <v>332</v>
+      </c>
+      <c r="B166" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="B167" t="s">
-        <v>329</v>
+        <v>165</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B168" t="s">
-        <v>331</v>
+        <v>166</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B169" t="s">
-        <v>333</v>
+        <v>167</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B170" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A171" t="s">
-        <v>43</v>
-      </c>
-      <c r="B171" t="s">
-        <v>336</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
general update to files
</commit_message>
<xml_diff>
--- a/Avantis Mapping/SPARQL_category.xlsx
+++ b/Avantis Mapping/SPARQL_category.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medney\Documents\GitHub\TWONTO\Avantis Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DC7112-BD60-4518-8089-E58BC443A36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052598AD-0AD9-4AAA-B0E9-BE61A201B454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{716C0CF8-2E33-46F2-BE6F-578AC5702A19}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{716C0CF8-2E33-46F2-BE6F-578AC5702A19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,19 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="359">
   <si>
     <t>TWONTO</t>
   </si>
   <si>
-    <t>UPS_x000D_
-Uninterruptible Power Supply</t>
-  </si>
-  <si>
-    <t>Collector,Circular_x000D_
-Collector,Helical Rotating</t>
-  </si>
-  <si>
     <t>Machine Tool,Planer</t>
   </si>
   <si>
@@ -58,16 +50,9 @@
     <t>Flocculator</t>
   </si>
   <si>
-    <t>Sensor,Security</t>
-  </si>
-  <si>
     <t>PPE,Lanyard</t>
   </si>
   <si>
-    <t>Relay_x000D_
-Relay,Protective</t>
-  </si>
-  <si>
     <t>Meter,Flow,Mass</t>
   </si>
   <si>
@@ -83,14 +68,6 @@
     <t>Switch,Temperature</t>
   </si>
   <si>
-    <t>Dust Control_x000D_
-Dust Control,Odour Control</t>
-  </si>
-  <si>
-    <t>Pressure Sensor_x000D_
-Sensor,Pressure</t>
-  </si>
-  <si>
     <t>RPU</t>
   </si>
   <si>
@@ -139,18 +116,6 @@
     <t>Flame Arrester</t>
   </si>
   <si>
-    <t>Cyclone_x000D_
-Classifier,Cyclone</t>
-  </si>
-  <si>
-    <t>Meter,Density_x000D_
-Analyzer,Density</t>
-  </si>
-  <si>
-    <t>Generator_x000D_
-Generator,Electricity</t>
-  </si>
-  <si>
     <t>Transmitter</t>
   </si>
   <si>
@@ -160,32 +125,12 @@
     <t>Lifting Device,Hoist</t>
   </si>
   <si>
-    <t>Agitator_x000D_
-Mixer</t>
-  </si>
-  <si>
-    <t>Motor Starter_x000D_
-Starter</t>
-  </si>
-  <si>
     <t>Network,Switch</t>
   </si>
   <si>
     <t>Weigh Scale</t>
   </si>
   <si>
-    <t>EntityCategory_x000D_
-Door</t>
-  </si>
-  <si>
-    <t>Drive,Variable Speed Electrical_x000D_
-Drive,Variable Speed Mechanical</t>
-  </si>
-  <si>
-    <t>Ultraviolet Disinfection_x000D_
-Ultraviolet Disinfection,System</t>
-  </si>
-  <si>
     <t>Meter,Flow</t>
   </si>
   <si>
@@ -228,10 +173,6 @@
     <t>Vacuum</t>
   </si>
   <si>
-    <t>Evaporator,Chlorine_x000D_
-Generator,Chlorine</t>
-  </si>
-  <si>
     <t>Conveyor,Belt</t>
   </si>
   <si>
@@ -244,23 +185,12 @@
     <t>Valve,Pressure Relief</t>
   </si>
   <si>
-    <t>Collector_x000D_
-Sludge Collector</t>
-  </si>
-  <si>
-    <t>Sensor,Motion_x000D_
-Switch,Motion</t>
-  </si>
-  <si>
     <t>Boiler</t>
   </si>
   <si>
     <t>Circuit Breaker</t>
   </si>
   <si>
-    <t>Analyzer,Residual Sulphite</t>
-  </si>
-  <si>
     <t>Analyzer,Chloramination</t>
   </si>
   <si>
@@ -285,27 +215,15 @@
     <t>Collector,Chain and Flight</t>
   </si>
   <si>
-    <t>Meter,Level_x000D_
-Transmitter,Level</t>
-  </si>
-  <si>
     <t>Capacitor</t>
   </si>
   <si>
     <t>Public Address System</t>
   </si>
   <si>
-    <t>Vessel_x000D_
-Vessel,Pressure</t>
-  </si>
-  <si>
     <t>H.V.A.C.,Air Conditioner</t>
   </si>
   <si>
-    <t>Power Pack_x000D_
-Power Pack,Hydraulic</t>
-  </si>
-  <si>
     <t>Heat Exchanger</t>
   </si>
   <si>
@@ -324,20 +242,9 @@
     <t>Meter,Sludge Blanket</t>
   </si>
   <si>
-    <t>Pump</t>
-  </si>
-  <si>
     <t>Vehicle</t>
   </si>
   <si>
-    <t>Valve,Safety_x000D_
-Valve,Safety,Act.</t>
-  </si>
-  <si>
-    <t>Valve,Backflow Preventer_x000D_
-Valve,Backflow Preventer,Reduced Pressure</t>
-  </si>
-  <si>
     <t>Analyzer,PH</t>
   </si>
   <si>
@@ -347,14 +254,6 @@
     <t>Machine Tool,Lathe</t>
   </si>
   <si>
-    <t>Blower_x000D_
-Fan</t>
-  </si>
-  <si>
-    <t>Meter,current_x000D_
-Meter,Power Recording</t>
-  </si>
-  <si>
     <t>Analyzer,Dissolved Oxygen (DO)</t>
   </si>
   <si>
@@ -373,9 +272,6 @@
     <t>Damper/Louver</t>
   </si>
   <si>
-    <t>Machine Tool,Drill Press</t>
-  </si>
-  <si>
     <t>Switch,Pressure</t>
   </si>
   <si>
@@ -397,27 +293,12 @@
     <t>Sampler</t>
   </si>
   <si>
-    <t>Analyzer,Suspended Solid_x000D_
-Meter,Suspended Solids</t>
-  </si>
-  <si>
-    <t>H.V.A.C.,Heater_x000D_
-Heater</t>
-  </si>
-  <si>
     <t>Meter,Flow,Displacement</t>
   </si>
   <si>
     <t>Clarifier</t>
   </si>
   <si>
-    <t>Comminutor_x000D_
-Grinder</t>
-  </si>
-  <si>
-    <t>Control Panel,Power Distribution Panel</t>
-  </si>
-  <si>
     <t>Screen</t>
   </si>
   <si>
@@ -430,20 +311,9 @@
     <t>Collector,Bridge</t>
   </si>
   <si>
-    <t>Atmosphere Monitoring Device,Stationary_x000D_
-Atmosphere Monitoring Device</t>
-  </si>
-  <si>
-    <t>Meter,Flow,Doppler_x000D_
-Meter,Flow,Ultrasonic</t>
-  </si>
-  <si>
     <t>Analyzer,Ammonia</t>
   </si>
   <si>
-    <t>Safety,Rupture Disc</t>
-  </si>
-  <si>
     <t>Server</t>
   </si>
   <si>
@@ -453,9 +323,6 @@
     <t>H.V.A.C.,Chiller</t>
   </si>
   <si>
-    <t>Switchgear</t>
-  </si>
-  <si>
     <t>Compressor</t>
   </si>
   <si>
@@ -465,15 +332,6 @@
     <t>Safety,Emergency Kit</t>
   </si>
   <si>
-    <t>Gate_x000D_
-Gate,Sluice_x000D_
-Gate,Sluice,Act._x000D_
-Valve,Gate,Sluice_x000D_
-Valve,Gate,Sluice,Act._x000D_
-Valve,Sluice Gate_x000D_
-Valve,Sluice Gate,Act.</t>
-  </si>
-  <si>
     <t>Crane</t>
   </si>
   <si>
@@ -528,10 +386,6 @@
     <t>PPE,Harness</t>
   </si>
   <si>
-    <t>Transmitter,Temperature_x000D_
-Meter,Temperature</t>
-  </si>
-  <si>
     <t>Analyzer,Fluoride</t>
   </si>
   <si>
@@ -544,11 +398,6 @@
     <t>Gearbox</t>
   </si>
   <si>
-    <t>Recorder_x000D_
-Recorder,Paper_x000D_
-Recorder,Paperless</t>
-  </si>
-  <si>
     <t>Control Panel,Lighting</t>
   </si>
   <si>
@@ -564,10 +413,6 @@
     <t>Transformer</t>
   </si>
   <si>
-    <t>PPE,Eyewash Station_x000D_
-Safety, Eye wash</t>
-  </si>
-  <si>
     <t>Gas Well</t>
   </si>
   <si>
@@ -589,150 +434,33 @@
     <t>UPS</t>
   </si>
   <si>
-    <t>rotating_collector</t>
-  </si>
-  <si>
     <t>planer</t>
   </si>
   <si>
     <t>controller</t>
   </si>
   <si>
-    <t>flocculation_tank</t>
-  </si>
-  <si>
-    <t>security_motion_sensor</t>
-  </si>
-  <si>
-    <t>fall_protection_energy_absorber</t>
-  </si>
-  <si>
-    <t>protection_relay</t>
-  </si>
-  <si>
-    <t>mass_flow_meter</t>
-  </si>
-  <si>
-    <t>automatic_external_defibrillator</t>
-  </si>
-  <si>
     <t>manhole</t>
   </si>
   <si>
     <t>PLC</t>
   </si>
   <si>
-    <t>temperature_switch</t>
-  </si>
-  <si>
-    <t>dust_collector</t>
-  </si>
-  <si>
-    <t>pressure_sensor_element</t>
-  </si>
-  <si>
-    <t>RTU</t>
-  </si>
-  <si>
-    <t>flow_switch</t>
-  </si>
-  <si>
-    <t>large_stationary_tool</t>
-  </si>
-  <si>
     <t>computer</t>
   </si>
   <si>
-    <t>roll_up_door</t>
-  </si>
-  <si>
-    <t>ozone_analyzer</t>
-  </si>
-  <si>
-    <t>level_switch</t>
-  </si>
-  <si>
     <t>elevator</t>
   </si>
   <si>
-    <t>fire_rated_door</t>
-  </si>
-  <si>
-    <t>level_sensor_element</t>
-  </si>
-  <si>
     <t>jointer</t>
   </si>
   <si>
-    <t>UV_disinfection_lamp_unit</t>
-  </si>
-  <si>
-    <t>air_scrubber</t>
-  </si>
-  <si>
-    <t>storage_tank</t>
-  </si>
-  <si>
-    <t>radial_arm_drill</t>
-  </si>
-  <si>
-    <t>flame_arrestor</t>
-  </si>
-  <si>
-    <t>cyclone_classifier</t>
-  </si>
-  <si>
-    <t>slude_density_meter</t>
-  </si>
-  <si>
     <t>generator-set</t>
   </si>
   <si>
-    <t>instrument_transmitter</t>
-  </si>
-  <si>
-    <t>first_aid_kit</t>
-  </si>
-  <si>
-    <t>lifting_equipment_hoist</t>
-  </si>
-  <si>
-    <t>mixer_or_agitator</t>
-  </si>
-  <si>
-    <t>motor_starter</t>
-  </si>
-  <si>
-    <t>network_switch</t>
-  </si>
-  <si>
-    <t>weight_scale</t>
-  </si>
-  <si>
-    <t>controlled_door_access</t>
-  </si>
-  <si>
     <t>VSD</t>
   </si>
   <si>
-    <t>UV_disinfection_assembly</t>
-  </si>
-  <si>
-    <t>flow_transmitter</t>
-  </si>
-  <si>
-    <t>spill_kit</t>
-  </si>
-  <si>
-    <t>ultraviolet_analyzer</t>
-  </si>
-  <si>
-    <t>still_or_video_mobile_camera</t>
-  </si>
-  <si>
-    <t>reservoir_tank</t>
-  </si>
-  <si>
     <t>forklift</t>
   </si>
   <si>
@@ -742,102 +470,21 @@
     <t>VFD</t>
   </si>
   <si>
-    <t>cable_segment</t>
-  </si>
-  <si>
-    <t>turbidity_analyzer</t>
-  </si>
-  <si>
-    <t>cooling_tower</t>
-  </si>
-  <si>
-    <t>equipment_or_access_chamber</t>
-  </si>
-  <si>
-    <t>ventilation_system</t>
-  </si>
-  <si>
-    <t>vacuum_cleaner</t>
-  </si>
-  <si>
-    <t>chlorinator_system</t>
-  </si>
-  <si>
-    <t>belt_conveyor</t>
-  </si>
-  <si>
-    <t>outfall_or_discharge_point</t>
-  </si>
-  <si>
-    <t>network_router</t>
-  </si>
-  <si>
-    <t>relief_valve</t>
-  </si>
-  <si>
-    <t>collector_mechanism</t>
-  </si>
-  <si>
-    <t>motion_sensor_element</t>
-  </si>
-  <si>
     <t>boiler</t>
   </si>
   <si>
     <t>breaker</t>
   </si>
   <si>
-    <t>sulphite_analyzer</t>
-  </si>
-  <si>
-    <t>chloramination_analyzer</t>
-  </si>
-  <si>
     <t>classifier</t>
   </si>
   <si>
-    <t>annunciator_panel</t>
-  </si>
-  <si>
     <t>motor</t>
   </si>
   <si>
-    <t>orp_analyzer</t>
-  </si>
-  <si>
-    <t>milling_machine</t>
-  </si>
-  <si>
-    <t>differential_pressure</t>
-  </si>
-  <si>
-    <t>chain_and_flight_collector</t>
-  </si>
-  <si>
-    <t>level_transmitter</t>
-  </si>
-  <si>
     <t>capacitor</t>
   </si>
   <si>
-    <t>public_annoucement_speaker</t>
-  </si>
-  <si>
-    <t>pressure_vessel</t>
-  </si>
-  <si>
-    <t>air_condition</t>
-  </si>
-  <si>
-    <t>hydraulic_power_pack</t>
-  </si>
-  <si>
-    <t>heat_exchanger</t>
-  </si>
-  <si>
-    <t>welding_receptacle</t>
-  </si>
-  <si>
     <t>boat</t>
   </si>
   <si>
@@ -847,244 +494,634 @@
     <t>engine</t>
   </si>
   <si>
-    <t>sludge_blanket_analyzer</t>
-  </si>
-  <si>
-    <t>pump_-_without_drive</t>
-  </si>
-  <si>
-    <t>passenger_vehicles</t>
-  </si>
-  <si>
-    <t>safety_valve</t>
-  </si>
-  <si>
-    <t>backflow_preventer</t>
-  </si>
-  <si>
-    <t>PH_analyzer</t>
-  </si>
-  <si>
-    <t>vibration_analyzer</t>
-  </si>
-  <si>
     <t>lathe</t>
   </si>
   <si>
     <t>blower</t>
   </si>
   <si>
-    <t>electrical_current_sensing_instrument</t>
-  </si>
-  <si>
-    <t>dissolved_oxygen_analyzer</t>
-  </si>
-  <si>
-    <t>pipe_segment</t>
-  </si>
-  <si>
-    <t>screw_conveyor</t>
-  </si>
-  <si>
-    <t>pressure_transmitter</t>
-  </si>
-  <si>
     <t>incinerator</t>
   </si>
   <si>
-    <t>air_damper</t>
-  </si>
-  <si>
-    <t>drill_press</t>
-  </si>
-  <si>
-    <t>pressure_switch</t>
-  </si>
-  <si>
     <t>centrifuge</t>
   </si>
   <si>
     <t>dryer</t>
   </si>
   <si>
-    <t>SCADA_computer_terminal</t>
-  </si>
-  <si>
-    <t>process_control_panel</t>
-  </si>
-  <si>
-    <t>rubber_insulating_gloves</t>
-  </si>
-  <si>
-    <t>auto_sampler</t>
-  </si>
-  <si>
-    <t>total_suspended_solids_analyzer</t>
-  </si>
-  <si>
     <t>heater</t>
   </si>
   <si>
-    <t>positive_displacement_flow_elements</t>
-  </si>
-  <si>
     <t>clarifier</t>
   </si>
   <si>
-    <t>grinder_or_comminutor</t>
-  </si>
-  <si>
-    <t>600V_insulated_case_electrical_cabinet</t>
-  </si>
-  <si>
     <t>screen</t>
   </si>
   <si>
-    <t>instrument_element</t>
-  </si>
-  <si>
-    <t>position_transmitter</t>
-  </si>
-  <si>
-    <t>travelling_bridge_collector</t>
-  </si>
-  <si>
-    <t>fixed_gas_detector</t>
-  </si>
-  <si>
-    <t>ultrasonic_flow_meter</t>
-  </si>
-  <si>
-    <t>ammonia_analyzer</t>
-  </si>
-  <si>
-    <t>rupture_disc</t>
-  </si>
-  <si>
-    <t>server_appliance</t>
-  </si>
-  <si>
-    <t>ozone_generator</t>
-  </si>
-  <si>
     <t>chiller</t>
   </si>
   <si>
-    <t>5kV_electrical_cabinet</t>
-  </si>
-  <si>
     <t>compressor</t>
   </si>
   <si>
-    <t>table_saw</t>
-  </si>
-  <si>
-    <t>channel_gate</t>
-  </si>
-  <si>
     <t>crane</t>
   </si>
   <si>
-    <t>self-contained_breathing_apparatus</t>
-  </si>
-  <si>
     <t>conveyor</t>
   </si>
   <si>
-    <t>lighting_unit</t>
-  </si>
-  <si>
     <t>dehumidifier</t>
   </si>
   <si>
-    <t>elevated_water_tank</t>
-  </si>
-  <si>
     <t>magmeter</t>
   </si>
   <si>
     <t>compactor</t>
   </si>
   <si>
-    <t>temperature_sensor_element</t>
-  </si>
-  <si>
-    <t>security_camera</t>
-  </si>
-  <si>
-    <t>hot_water_tank</t>
-  </si>
-  <si>
     <t>venturi</t>
   </si>
   <si>
     <t>strainer</t>
   </si>
   <si>
-    <t>torque_switch</t>
-  </si>
-  <si>
-    <t>chlorine_analyzer</t>
-  </si>
-  <si>
-    <t>orthophosphate_analyzer</t>
-  </si>
-  <si>
-    <t>ash_lagoon</t>
-  </si>
-  <si>
-    <t>fall_arrest_harness</t>
-  </si>
-  <si>
-    <t>temperature_transmitter</t>
-  </si>
-  <si>
-    <t>fluoride_analyzer</t>
-  </si>
-  <si>
-    <t>check_valve</t>
-  </si>
-  <si>
-    <t>position_switch</t>
-  </si>
-  <si>
     <t>gearbox</t>
   </si>
   <si>
-    <t>data_logger</t>
-  </si>
-  <si>
-    <t>120V-208V_electrical_panel</t>
-  </si>
-  <si>
-    <t>flow_sensor_element</t>
-  </si>
-  <si>
-    <t>humidier</t>
-  </si>
-  <si>
     <t>well</t>
   </si>
   <si>
     <t>transformer</t>
   </si>
   <si>
-    <t>emergency_eyewash</t>
-  </si>
-  <si>
-    <t>gas_holder</t>
-  </si>
-  <si>
-    <t>granular_material</t>
-  </si>
-  <si>
-    <t>bar_screen_unit</t>
-  </si>
-  <si>
-    <t>screw_classifier</t>
-  </si>
-  <si>
-    <t>position_sensing_instrument</t>
+    <t>auto sampler</t>
+  </si>
+  <si>
+    <t>radial arm drill</t>
+  </si>
+  <si>
+    <t>pressure sensor element</t>
+  </si>
+  <si>
+    <t>Pressure Sensor</t>
+  </si>
+  <si>
+    <t>air damper</t>
+  </si>
+  <si>
+    <t>level transmitter</t>
+  </si>
+  <si>
+    <t>Transmitter,Level</t>
+  </si>
+  <si>
+    <t>PH analyzer</t>
+  </si>
+  <si>
+    <t>fire rated door</t>
+  </si>
+  <si>
+    <t>UV disinfection lamp unit</t>
+  </si>
+  <si>
+    <t>vibration analyzer</t>
+  </si>
+  <si>
+    <t>pressure vessel</t>
+  </si>
+  <si>
+    <t>Vessel</t>
+  </si>
+  <si>
+    <t>ventilation system</t>
+  </si>
+  <si>
+    <t>data logger</t>
+  </si>
+  <si>
+    <t>Recorder,Paperless</t>
+  </si>
+  <si>
+    <t>flow sensor element</t>
+  </si>
+  <si>
+    <t>flow switch</t>
+  </si>
+  <si>
+    <t>flow transmitter</t>
+  </si>
+  <si>
+    <t>lifting equipment hoist</t>
+  </si>
+  <si>
+    <t>elevated water tank</t>
+  </si>
+  <si>
+    <t>mixer or agitator</t>
+  </si>
+  <si>
+    <t>Agitator</t>
+  </si>
+  <si>
+    <t>pressure switch</t>
+  </si>
+  <si>
+    <t>pressure transmitter</t>
+  </si>
+  <si>
+    <t>spill kit</t>
+  </si>
+  <si>
+    <t>channel gate</t>
+  </si>
+  <si>
+    <t>Valve,Sluice Gate,Act.</t>
+  </si>
+  <si>
+    <t>protection relay</t>
+  </si>
+  <si>
+    <t>Relay,Protective</t>
+  </si>
+  <si>
+    <t>weight scale</t>
+  </si>
+  <si>
+    <t>ultrasonic flow meter</t>
+  </si>
+  <si>
+    <t>Meter,Flow,Ultrasonic</t>
+  </si>
+  <si>
+    <t>Mixer</t>
+  </si>
+  <si>
+    <t>positive displacement flow elements</t>
+  </si>
+  <si>
+    <t>orthophosphate analyzer</t>
+  </si>
+  <si>
+    <t>flowmeter</t>
+  </si>
+  <si>
+    <t>safety valve</t>
+  </si>
+  <si>
+    <t>Valve,Safety,Act.</t>
+  </si>
+  <si>
+    <t>fluoride analyzer</t>
+  </si>
+  <si>
+    <t>self-contained breathing apparatus</t>
+  </si>
+  <si>
+    <t>Drive,Variable Speed Electrical</t>
+  </si>
+  <si>
+    <t>ash lagoon</t>
+  </si>
+  <si>
+    <t>ultraviolet analyzer</t>
+  </si>
+  <si>
+    <t>Blower</t>
+  </si>
+  <si>
+    <t>fall protection energy absorber</t>
+  </si>
+  <si>
+    <t>emergency eyewash</t>
+  </si>
+  <si>
+    <t>PPE,Eyewash Station</t>
+  </si>
+  <si>
+    <t>vacuum cleaner</t>
+  </si>
+  <si>
+    <t>relief valve</t>
+  </si>
+  <si>
+    <t>milling machine</t>
+  </si>
+  <si>
+    <t>Valve,Gate,Sluice</t>
+  </si>
+  <si>
+    <t>Valve,Gate,Sluice,Act.</t>
+  </si>
+  <si>
+    <t>Valve,Sluice Gate</t>
+  </si>
+  <si>
+    <t>controlled door access</t>
+  </si>
+  <si>
+    <t>Door</t>
+  </si>
+  <si>
+    <t>Relay</t>
+  </si>
+  <si>
+    <t>rotating collector</t>
+  </si>
+  <si>
+    <t>Collector,Circular</t>
+  </si>
+  <si>
+    <t>dissolved oxygen analyzer</t>
+  </si>
+  <si>
+    <t>outfall or discharge point</t>
+  </si>
+  <si>
+    <t>process control panel</t>
+  </si>
+  <si>
+    <t>gas holder</t>
+  </si>
+  <si>
+    <t>check valve</t>
+  </si>
+  <si>
+    <t>tanked hot water heater</t>
+  </si>
+  <si>
+    <t>operator interface terminal</t>
+  </si>
+  <si>
+    <t>Vessel,Pressure</t>
+  </si>
+  <si>
+    <t>mass flow meter</t>
+  </si>
+  <si>
+    <t>Gate</t>
+  </si>
+  <si>
+    <t>storage tank</t>
+  </si>
+  <si>
+    <t>motor starter</t>
+  </si>
+  <si>
+    <t>Starter</t>
+  </si>
+  <si>
+    <t>Drive,Variable Speed Mechanical</t>
+  </si>
+  <si>
+    <t>fixed gas detector</t>
+  </si>
+  <si>
+    <t>Atmosphere Monitoring Device,Stationary</t>
+  </si>
+  <si>
+    <t>Gate,Sluice,Act.</t>
+  </si>
+  <si>
+    <t>flame arrestor</t>
+  </si>
+  <si>
+    <t>EntityCategory</t>
+  </si>
+  <si>
+    <t>annunciator panel</t>
+  </si>
+  <si>
+    <t>network switch</t>
+  </si>
+  <si>
+    <t>pipe segment</t>
+  </si>
+  <si>
+    <t>instrument sensor element</t>
+  </si>
+  <si>
+    <t>hydraulic power pack</t>
+  </si>
+  <si>
+    <t>Power Pack,Hydraulic</t>
+  </si>
+  <si>
+    <t>position sensing instrument</t>
+  </si>
+  <si>
+    <t>Sensor,Pressure</t>
+  </si>
+  <si>
+    <t>heat exchanger</t>
+  </si>
+  <si>
+    <t>screw conveyor</t>
+  </si>
+  <si>
+    <t>bar screen unit</t>
+  </si>
+  <si>
+    <t>Generator</t>
+  </si>
+  <si>
+    <t>cyclone classifier</t>
+  </si>
+  <si>
+    <t>Classifier,Cyclone</t>
+  </si>
+  <si>
+    <t>network router</t>
+  </si>
+  <si>
+    <t>screw classifier</t>
+  </si>
+  <si>
+    <t>ozone generator</t>
+  </si>
+  <si>
+    <t>Cyclone</t>
+  </si>
+  <si>
+    <t>Collector,Helical Rotating</t>
+  </si>
+  <si>
+    <t>temperature sensor element</t>
+  </si>
+  <si>
+    <t>dust collector</t>
+  </si>
+  <si>
+    <t>Dust Control,Odour Control</t>
+  </si>
+  <si>
+    <t>level switch</t>
+  </si>
+  <si>
+    <t>security camera</t>
+  </si>
+  <si>
+    <t>slude density meter</t>
+  </si>
+  <si>
+    <t>Meter,Density</t>
+  </si>
+  <si>
+    <t>fall arrest harness</t>
+  </si>
+  <si>
+    <t>chlorinator system</t>
+  </si>
+  <si>
+    <t>Generator,Chlorine</t>
+  </si>
+  <si>
+    <t>server appliance</t>
+  </si>
+  <si>
+    <t>flocculation tank</t>
+  </si>
+  <si>
+    <t>rubber insulating gloves</t>
+  </si>
+  <si>
+    <t>Safety, Eye wash</t>
+  </si>
+  <si>
+    <t>reservoir tank</t>
+  </si>
+  <si>
+    <t>differential pressure</t>
+  </si>
+  <si>
+    <t>still or video mobile camera</t>
+  </si>
+  <si>
+    <t>temperature switch</t>
+  </si>
+  <si>
+    <t>humidifier</t>
+  </si>
+  <si>
+    <t>passenger vehicle</t>
+  </si>
+  <si>
+    <t>first aid kit</t>
+  </si>
+  <si>
+    <t>Recorder,Paper</t>
+  </si>
+  <si>
+    <t>Atmosphere Monitoring Device</t>
+  </si>
+  <si>
+    <t>chloramination analyzer</t>
+  </si>
+  <si>
+    <t>grinder or comminutor</t>
+  </si>
+  <si>
+    <t>Grinder</t>
+  </si>
+  <si>
+    <t>H.V.A.C.,Heater</t>
+  </si>
+  <si>
+    <t>UV disinfection assembly</t>
+  </si>
+  <si>
+    <t>Ultraviolet Disinfection</t>
+  </si>
+  <si>
+    <t>Power Pack</t>
+  </si>
+  <si>
+    <t>Meter,Level</t>
+  </si>
+  <si>
+    <t>sludge blanket analyzer</t>
+  </si>
+  <si>
+    <t>Dust Control</t>
+  </si>
+  <si>
+    <t>Motor Starter</t>
+  </si>
+  <si>
+    <t>motion sensor element</t>
+  </si>
+  <si>
+    <t>Switch,Motion</t>
+  </si>
+  <si>
+    <t>cooling tower</t>
+  </si>
+  <si>
+    <t>travelling bridge collector</t>
+  </si>
+  <si>
+    <t>total suspended solids analyzer</t>
+  </si>
+  <si>
+    <t>Meter,Suspended Solids</t>
+  </si>
+  <si>
+    <t>equipment or access chamber</t>
+  </si>
+  <si>
+    <t>granular material</t>
+  </si>
+  <si>
+    <t>Fan</t>
+  </si>
+  <si>
+    <t>position switch</t>
+  </si>
+  <si>
+    <t>position transmitter</t>
+  </si>
+  <si>
+    <t>electrical current sensing instrument</t>
+  </si>
+  <si>
+    <t>Meter,Power Recording</t>
+  </si>
+  <si>
+    <t>belt conveyor</t>
+  </si>
+  <si>
+    <t>public annoucement speaker</t>
+  </si>
+  <si>
+    <t>Valve,Safety</t>
+  </si>
+  <si>
+    <t>Recorder</t>
+  </si>
+  <si>
+    <t>welding receptacle</t>
+  </si>
+  <si>
+    <t>Ultraviolet Disinfection,System</t>
+  </si>
+  <si>
+    <t>automatic external defibrillator</t>
+  </si>
+  <si>
+    <t>Meter,Flow,Doppler</t>
+  </si>
+  <si>
+    <t>cable segment</t>
+  </si>
+  <si>
+    <t>turbidity analyzer</t>
+  </si>
+  <si>
+    <t>collector mechanism</t>
+  </si>
+  <si>
+    <t>Sludge Collector</t>
+  </si>
+  <si>
+    <t>Evaporator,Chlorine</t>
+  </si>
+  <si>
+    <t>ozone analyzer</t>
+  </si>
+  <si>
+    <t>Analyzer,Suspended Solid</t>
+  </si>
+  <si>
+    <t>Uninterruptible Power Supply</t>
+  </si>
+  <si>
+    <t>torque switch</t>
+  </si>
+  <si>
+    <t>Comminutor</t>
+  </si>
+  <si>
+    <t>Generator,Electricity</t>
+  </si>
+  <si>
+    <t>instrument transmitter</t>
+  </si>
+  <si>
+    <t>ammonia analyzer</t>
+  </si>
+  <si>
+    <t>roll up door</t>
+  </si>
+  <si>
+    <t>level sensor element</t>
+  </si>
+  <si>
+    <t>lighting unit</t>
+  </si>
+  <si>
+    <t>Meter,current</t>
+  </si>
+  <si>
+    <t>chlorine analyzer</t>
+  </si>
+  <si>
+    <t>Collector</t>
+  </si>
+  <si>
+    <t>RTU panel</t>
+  </si>
+  <si>
+    <t>LV electrical panel</t>
+  </si>
+  <si>
+    <t>air scrubber</t>
+  </si>
+  <si>
+    <t>Analyzer,Density</t>
+  </si>
+  <si>
+    <t>backflow preventer</t>
+  </si>
+  <si>
+    <t>Valve,Backflow Preventer,Reduced Pressure</t>
+  </si>
+  <si>
+    <t>large stationary tool</t>
+  </si>
+  <si>
+    <t>Sensor,Motion</t>
+  </si>
+  <si>
+    <t>Gate,Sluice</t>
+  </si>
+  <si>
+    <t>table saw</t>
+  </si>
+  <si>
+    <t>ORP analyzer</t>
+  </si>
+  <si>
+    <t>Heater</t>
+  </si>
+  <si>
+    <t>chain and flight collector</t>
+  </si>
+  <si>
+    <t>Valve,Backflow Preventer</t>
+  </si>
+  <si>
+    <t>air condition</t>
+  </si>
+  <si>
+    <t>PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX tw: &lt;http://www.toronto.ca/TWONTO#&gt;
+SELECT (STR(?label) as ?TWONTO) (STR(?object) as ?Avantis)
+WHERE { 
+    ?entityIRI tw:is_equivalent_to_Avantis_category ?object ;
+              rdfs:label ?label .
+}</t>
   </si>
 </sst>
 </file>
@@ -1200,8 +1237,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{95B7462F-2E77-4297-9361-348E17AE61B7}" name="Table1" displayName="Table1" ref="A2:B170" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A2:B170" xr:uid="{95B7462F-2E77-4297-9361-348E17AE61B7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{95B7462F-2E77-4297-9361-348E17AE61B7}" name="Table1" displayName="Table1" ref="A2:B205" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A2:B205" xr:uid="{95B7462F-2E77-4297-9361-348E17AE61B7}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{F929C49D-2775-4718-8C6D-B5829C8CADDE}" name="TWONTO"/>
     <tableColumn id="2" xr3:uid="{69FF631B-786D-4A8E-A604-FCCAC8BACC05}" name="Category"/>
@@ -1507,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C799550E-49B1-4512-9CC1-86876BA1337E}">
-  <dimension ref="A2:B170"/>
+  <dimension ref="A1:B205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1519,612 +1556,617 @@
     <col min="2" max="2" width="61.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>4</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>20</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>201</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>196</v>
+        <v>148</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>29</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>167</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>208</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>201</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>202</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>206</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>208</v>
+        <v>140</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>39</v>
+        <v>213</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>211</v>
+        <v>153</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>212</v>
+        <v>160</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>219</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>218</v>
+        <v>133</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>220</v>
+        <v>154</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>224</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>222</v>
+        <v>155</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>55</v>
+        <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>228</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>226</v>
+        <v>156</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B60" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B63" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B64" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B65" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>235</v>
+        <v>150</v>
       </c>
       <c r="B68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>236</v>
+        <v>183</v>
       </c>
       <c r="B69" t="s">
-        <v>67</v>
+        <v>238</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B70" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>238</v>
+        <v>198</v>
       </c>
       <c r="B71" t="s">
-        <v>69</v>
+        <v>240</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>239</v>
+        <v>135</v>
       </c>
       <c r="B72" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B73" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B74" t="s">
-        <v>72</v>
+        <v>243</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>242</v>
+        <v>197</v>
       </c>
       <c r="B75" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>243</v>
+        <v>162</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
+        <v>140</v>
+      </c>
+      <c r="B77" t="s">
         <v>244</v>
-      </c>
-      <c r="B77" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
@@ -2132,23 +2174,23 @@
         <v>245</v>
       </c>
       <c r="B78" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>77</v>
+        <v>247</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>247</v>
+        <v>144</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
@@ -2156,15 +2198,15 @@
         <v>248</v>
       </c>
       <c r="B81" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>226</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -2172,47 +2214,47 @@
         <v>250</v>
       </c>
       <c r="B83" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>251</v>
+        <v>146</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B85" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B86" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
+        <v>254</v>
+      </c>
+      <c r="B88" t="s">
         <v>255</v>
-      </c>
-      <c r="B88" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
@@ -2220,15 +2262,15 @@
         <v>256</v>
       </c>
       <c r="B89" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>174</v>
+      </c>
+      <c r="B90" t="s">
         <v>257</v>
-      </c>
-      <c r="B90" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
@@ -2236,7 +2278,7 @@
         <v>258</v>
       </c>
       <c r="B91" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
@@ -2244,23 +2286,23 @@
         <v>259</v>
       </c>
       <c r="B92" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>260</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
+        <v>139</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
@@ -2268,55 +2310,55 @@
         <v>262</v>
       </c>
       <c r="B95" t="s">
-        <v>93</v>
+        <v>263</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B96" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B97" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>266</v>
+        <v>131</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
+        <v>262</v>
+      </c>
+      <c r="B100" t="s">
         <v>267</v>
-      </c>
-      <c r="B100" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
+        <v>229</v>
+      </c>
+      <c r="B101" t="s">
         <v>268</v>
-      </c>
-      <c r="B101" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
@@ -2324,7 +2366,7 @@
         <v>269</v>
       </c>
       <c r="B102" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
@@ -2332,23 +2374,23 @@
         <v>270</v>
       </c>
       <c r="B103" t="s">
-        <v>101</v>
+        <v>271</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B104" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>272</v>
+        <v>188</v>
       </c>
       <c r="B105" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
@@ -2356,7 +2398,7 @@
         <v>273</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
@@ -2364,39 +2406,39 @@
         <v>274</v>
       </c>
       <c r="B107" t="s">
-        <v>105</v>
+        <v>275</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>275</v>
+        <v>142</v>
       </c>
       <c r="B108" t="s">
-        <v>106</v>
+        <v>37</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>276</v>
+        <v>142</v>
       </c>
       <c r="B109" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B110" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
+        <v>277</v>
+      </c>
+      <c r="B111" t="s">
         <v>278</v>
-      </c>
-      <c r="B111" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
@@ -2404,7 +2446,7 @@
         <v>279</v>
       </c>
       <c r="B112" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -2412,463 +2454,743 @@
         <v>280</v>
       </c>
       <c r="B113" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
+        <v>145</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
         <v>281</v>
       </c>
-      <c r="B114" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
-        <v>282</v>
-      </c>
       <c r="B115" s="3" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>283</v>
+        <v>218</v>
       </c>
       <c r="B116" t="s">
-        <v>114</v>
+        <v>282</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B117" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>285</v>
+        <v>134</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B119" t="s">
-        <v>117</v>
+        <v>57</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>287</v>
+        <v>158</v>
       </c>
       <c r="B120" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B121" t="s">
-        <v>119</v>
+        <v>34</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B122" t="s">
-        <v>120</v>
+        <v>9</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B123" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>123</v>
+        <v>27</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>293</v>
+        <v>186</v>
       </c>
       <c r="B126" t="s">
-        <v>124</v>
+        <v>290</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>294</v>
+        <v>245</v>
       </c>
       <c r="B127" t="s">
-        <v>125</v>
+        <v>291</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B128" t="s">
-        <v>126</v>
+        <v>51</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B129" t="s">
-        <v>127</v>
+        <v>294</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>297</v>
+        <v>157</v>
       </c>
       <c r="B130" t="s">
-        <v>128</v>
+        <v>295</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>298</v>
+        <v>171</v>
       </c>
       <c r="B131" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>299</v>
+        <v>147</v>
       </c>
       <c r="B132" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>300</v>
+        <v>147</v>
       </c>
       <c r="B133" t="s">
-        <v>131</v>
+        <v>54</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>215</v>
+        <v>296</v>
       </c>
       <c r="B134" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>301</v>
+        <v>254</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>133</v>
+        <v>298</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>302</v>
+        <v>177</v>
       </c>
       <c r="B136" t="s">
-        <v>134</v>
+        <v>299</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B137" t="s">
-        <v>135</v>
+        <v>67</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>304</v>
+        <v>270</v>
       </c>
       <c r="B138" t="s">
-        <v>136</v>
+        <v>301</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>305</v>
+        <v>159</v>
       </c>
       <c r="B139" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>306</v>
+        <v>242</v>
       </c>
       <c r="B140" t="s">
-        <v>138</v>
+        <v>302</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B141" t="s">
-        <v>139</v>
+        <v>304</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B142" t="s">
-        <v>140</v>
+        <v>41</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B143" t="s">
-        <v>141</v>
+        <v>90</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>310</v>
+        <v>137</v>
       </c>
       <c r="B144" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B145" t="s">
-        <v>143</v>
+        <v>308</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B146" t="s">
-        <v>144</v>
+        <v>42</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>313</v>
+        <v>141</v>
       </c>
       <c r="B147" t="s">
-        <v>145</v>
+        <v>36</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B148" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>315</v>
+        <v>153</v>
       </c>
       <c r="B149" t="s">
-        <v>147</v>
+        <v>311</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B150" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B151" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B152" t="s">
-        <v>150</v>
+        <v>315</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>319</v>
+        <v>161</v>
       </c>
       <c r="B153" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>152</v>
+        <v>45</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B155" t="s">
-        <v>153</v>
+        <v>60</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>322</v>
+        <v>209</v>
       </c>
       <c r="B156" t="s">
-        <v>154</v>
+        <v>318</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>323</v>
+        <v>186</v>
       </c>
       <c r="B157" t="s">
-        <v>155</v>
+        <v>319</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B158" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>325</v>
+        <v>296</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>157</v>
+        <v>321</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B160" t="s">
-        <v>158</v>
+        <v>6</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>327</v>
+        <v>149</v>
       </c>
       <c r="B161" t="s">
-        <v>159</v>
+        <v>64</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>328</v>
+        <v>203</v>
       </c>
       <c r="B162" t="s">
-        <v>160</v>
+        <v>323</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B163" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B164" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>332</v>
+        <v>277</v>
       </c>
       <c r="B166" t="s">
-        <v>164</v>
+        <v>328</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>333</v>
+        <v>169</v>
       </c>
       <c r="B167" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B168" t="s">
-        <v>166</v>
+        <v>15</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>335</v>
+        <v>307</v>
       </c>
       <c r="B169" t="s">
-        <v>167</v>
+        <v>330</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
+        <v>168</v>
+      </c>
+      <c r="B170" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>163</v>
+      </c>
+      <c r="B171" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>131</v>
+      </c>
+      <c r="B172" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>332</v>
+      </c>
+      <c r="B173" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>293</v>
+      </c>
+      <c r="B174" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>139</v>
+      </c>
+      <c r="B175" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>335</v>
+      </c>
+      <c r="B176" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
         <v>336</v>
       </c>
-      <c r="B170" t="s">
-        <v>168</v>
+      <c r="B177" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>151</v>
+      </c>
+      <c r="B178" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>337</v>
+      </c>
+      <c r="B179" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>338</v>
+      </c>
+      <c r="B180" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>339</v>
+      </c>
+      <c r="B181" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>314</v>
+      </c>
+      <c r="B182" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>341</v>
+      </c>
+      <c r="B183" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>326</v>
+      </c>
+      <c r="B184" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>343</v>
+      </c>
+      <c r="B185" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>344</v>
+      </c>
+      <c r="B186" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>132</v>
+      </c>
+      <c r="B187" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>345</v>
+      </c>
+      <c r="B188" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>274</v>
+      </c>
+      <c r="B189" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>170</v>
+      </c>
+      <c r="B190" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>189</v>
+      </c>
+      <c r="B191" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>347</v>
+      </c>
+      <c r="B192" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>349</v>
+      </c>
+      <c r="B193" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>303</v>
+      </c>
+      <c r="B194" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>152</v>
+      </c>
+      <c r="B195" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>136</v>
+      </c>
+      <c r="B196" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>143</v>
+      </c>
+      <c r="B197" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>198</v>
+      </c>
+      <c r="B198" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>352</v>
+      </c>
+      <c r="B199" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>353</v>
+      </c>
+      <c r="B200" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>157</v>
+      </c>
+      <c r="B201" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>166</v>
+      </c>
+      <c r="B202" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
+        <v>355</v>
+      </c>
+      <c r="B203" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>347</v>
+      </c>
+      <c r="B204" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
+        <v>357</v>
+      </c>
+      <c r="B205" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>